<commit_message>
added bicubic and bisteffen interpolation
</commit_message>
<xml_diff>
--- a/Distribution/Demo.xlsx
+++ b/Distribution/Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="5374" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="5374" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interpolation" sheetId="2" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="94">
   <si>
     <t>x</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t>Generates random sample on [0,1), using Mersenne Twister (MT19937)</t>
+  </si>
+  <si>
+    <t>bicubic</t>
+  </si>
+  <si>
+    <t>bicubicref</t>
+  </si>
+  <si>
+    <t>bisteffen</t>
   </si>
 </sst>
 </file>
@@ -934,6 +943,14 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
+    <main first="rtdsrv.a7a04b19a31a4c9eb642676ab37cf19a">
+      <tp t="e">
+        <v>#N/A</v>
+        <stp/>
+        <stp>e79a1697-4349-44b8-ac6d-0b0912bcaa2c</stp>
+        <tr r="I4" s="4"/>
+      </tp>
+    </main>
     <main first="rtdsrv.be1f78f34db74ce1ba29d9b8b6185772">
       <tp t="e">
         <v>#N/A</v>
@@ -949,8 +966,6 @@
         <stp>383aa482-d8e1-4289-873d-6d7cfaf34a0d</stp>
         <tr r="F5" s="2"/>
       </tp>
-    </main>
-    <main first="rtdsrv.666c2edb6b434254be57b404ebf65d1e">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
@@ -964,14 +979,6 @@
         <stp/>
         <stp>9a7c33f7-3632-4515-9bfc-15c25b54e5f1</stp>
         <tr r="D8" s="6"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.e41265aec3fd44b78717a1034b7d01cb">
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>d4c570c2-0388-453b-b684-cf29612bcc50</stp>
-        <tr r="I4" s="4"/>
       </tp>
     </main>
     <main first="rtdsrv.017addb0c58e4917a43bf64c27d6deb9">
@@ -6566,31 +6573,31 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96</c:v>
+                  <c:v>0.96160000000000012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92</c:v>
+                  <c:v>0.92479999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.88</c:v>
+                  <c:v>0.8872000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.84000000000000008</c:v>
+                  <c:v>0.84640000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.74</c:v>
+                  <c:v>0.73680000000000012</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68</c:v>
+                  <c:v>0.65839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.62</c:v>
+                  <c:v>0.58159999999999989</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.5232</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.5</c:v>
@@ -6675,37 +6682,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.9</c:v>
+                  <c:v>0.89100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.874</c:v>
+                  <c:v>0.86768560000000017</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84800000000000009</c:v>
+                  <c:v>0.84579680000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82199999999999995</c:v>
+                  <c:v>0.82319520000000013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79600000000000004</c:v>
+                  <c:v>0.79774240000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.77</c:v>
+                  <c:v>0.76730000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.72599999999999998</c:v>
+                  <c:v>0.72363280000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68200000000000005</c:v>
+                  <c:v>0.66816639999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.63800000000000001</c:v>
+                  <c:v>0.61325359999999984</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.59400000000000008</c:v>
+                  <c:v>0.57124719999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55449999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6787,37 +6794,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.8</c:v>
+                  <c:v>0.76800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78799999999999992</c:v>
+                  <c:v>0.76170880000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77600000000000002</c:v>
+                  <c:v>0.75664639999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76400000000000001</c:v>
+                  <c:v>0.75096960000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.752</c:v>
+                  <c:v>0.74283519999999992</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.74</c:v>
+                  <c:v>0.73040000000000016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.71199999999999997</c:v>
+                  <c:v>0.70877440000000014</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68400000000000005</c:v>
+                  <c:v>0.67918719999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.65600000000000003</c:v>
+                  <c:v>0.64897280000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.628</c:v>
+                  <c:v>0.62546559999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.6</c:v>
+                  <c:v>0.6160000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6899,37 +6906,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                  <c:v>0.63700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70199999999999996</c:v>
+                  <c:v>0.64883920000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70400000000000007</c:v>
+                  <c:v>0.6616976</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70599999999999996</c:v>
+                  <c:v>0.67404640000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.70800000000000007</c:v>
+                  <c:v>0.6843568000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71000000000000008</c:v>
+                  <c:v>0.69110000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.69799999999999995</c:v>
+                  <c:v>0.69294960000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68600000000000005</c:v>
+                  <c:v>0.69092480000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.67400000000000004</c:v>
+                  <c:v>0.68701520000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.66200000000000003</c:v>
+                  <c:v>0.6832104</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.65</c:v>
+                  <c:v>0.68149999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7011,37 +7018,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.6</c:v>
+                  <c:v>0.504</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61599999999999988</c:v>
+                  <c:v>0.53424640000000012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.63200000000000012</c:v>
+                  <c:v>0.5652992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64799999999999991</c:v>
+                  <c:v>0.59594880000000017</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66400000000000003</c:v>
+                  <c:v>0.62498560000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68</c:v>
+                  <c:v>0.65120000000000011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.68399999999999994</c:v>
+                  <c:v>0.67688320000000013</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68800000000000006</c:v>
+                  <c:v>0.70284159999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.69200000000000006</c:v>
+                  <c:v>0.72563839999999991</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.69600000000000006</c:v>
+                  <c:v>0.74183679999999985</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.7</c:v>
+                  <c:v>0.74799999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7123,37 +7130,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53</c:v>
+                  <c:v>0.42310000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.4718</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59</c:v>
+                  <c:v>0.52020000000000011</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.62000000000000011</c:v>
+                  <c:v>0.56740000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.65</c:v>
+                  <c:v>0.61250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.66999999999999993</c:v>
+                  <c:v>0.66130000000000011</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69</c:v>
+                  <c:v>0.71440000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.71</c:v>
+                  <c:v>0.7631</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.73</c:v>
+                  <c:v>0.79870000000000008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.75</c:v>
+                  <c:v>0.8125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7237,37 +7244,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.25600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44399999999999995</c:v>
+                  <c:v>0.32056960000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.48800000000000004</c:v>
+                  <c:v>0.38554879999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53200000000000003</c:v>
+                  <c:v>0.45032320000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57600000000000007</c:v>
+                  <c:v>0.51427840000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.62</c:v>
+                  <c:v>0.57679999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.65600000000000003</c:v>
+                  <c:v>0.64692480000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69199999999999995</c:v>
+                  <c:v>0.7250624</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.72799999999999998</c:v>
+                  <c:v>0.79765760000000008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.76400000000000001</c:v>
+                  <c:v>0.8511552</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.8</c:v>
+                  <c:v>0.87200000000000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7351,37 +7358,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.15300000000000008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35799999999999998</c:v>
+                  <c:v>0.23182480000000011</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41600000000000004</c:v>
+                  <c:v>0.31089440000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.47399999999999998</c:v>
+                  <c:v>0.38984160000000012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53200000000000003</c:v>
+                  <c:v>0.46829920000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59000000000000008</c:v>
+                  <c:v>0.54590000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.64200000000000002</c:v>
+                  <c:v>0.63448240000000011</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69399999999999995</c:v>
+                  <c:v>0.73429120000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.746</c:v>
+                  <c:v>0.8275688000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79800000000000004</c:v>
+                  <c:v>0.89655759999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.85</c:v>
+                  <c:v>0.92349999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7465,37 +7472,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.19999999999999996</c:v>
+                  <c:v>7.1999999999999981E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27199999999999991</c:v>
+                  <c:v>0.16203519999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34400000000000008</c:v>
+                  <c:v>0.25218560000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41599999999999993</c:v>
+                  <c:v>0.34227840000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48799999999999999</c:v>
+                  <c:v>0.43214080000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.52159999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.628</c:v>
+                  <c:v>0.62469760000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69599999999999995</c:v>
+                  <c:v>0.74154880000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.76400000000000001</c:v>
+                  <c:v>0.85109120000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.83200000000000007</c:v>
+                  <c:v>0.93226240000000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.9</c:v>
+                  <c:v>0.96399999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7579,37 +7586,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>9.9999999999999978E-2</c:v>
+                  <c:v>1.8999999999999989E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18599999999999994</c:v>
+                  <c:v>0.1163704</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.27200000000000002</c:v>
+                  <c:v>0.21377119999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35799999999999987</c:v>
+                  <c:v>0.31115680000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44400000000000001</c:v>
+                  <c:v>0.4084816</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.53</c:v>
+                  <c:v>0.50569999999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.61399999999999999</c:v>
+                  <c:v>0.61829520000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69799999999999995</c:v>
+                  <c:v>0.74629759999999989</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.78200000000000003</c:v>
+                  <c:v>0.8664824000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8660000000000001</c:v>
+                  <c:v>0.95562479999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.95</c:v>
+                  <c:v>0.99049999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7696,13 +7703,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9999999999999978E-2</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20000000000000007</c:v>
+                  <c:v>0.19999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.29999999999999993</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.4</c:v>
@@ -7711,16 +7718,16 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.6160000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7</c:v>
+                  <c:v>0.748</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8</c:v>
+                  <c:v>0.87200000000000011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.9</c:v>
+                  <c:v>0.96399999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
@@ -8263,31 +8270,31 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96</c:v>
+                  <c:v>0.96160000000000012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92</c:v>
+                  <c:v>0.92479999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.88</c:v>
+                  <c:v>0.8872000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.84000000000000008</c:v>
+                  <c:v>0.84640000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.74</c:v>
+                  <c:v>0.73680000000000012</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68</c:v>
+                  <c:v>0.65839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.62</c:v>
+                  <c:v>0.58159999999999989</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.56000000000000005</c:v>
+                  <c:v>0.5232</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.5</c:v>
@@ -8377,37 +8384,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.9</c:v>
+                  <c:v>0.89100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.874</c:v>
+                  <c:v>0.86768560000000017</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84800000000000009</c:v>
+                  <c:v>0.84579680000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82199999999999995</c:v>
+                  <c:v>0.82319520000000013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79600000000000004</c:v>
+                  <c:v>0.79774240000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.77</c:v>
+                  <c:v>0.76730000000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.72599999999999998</c:v>
+                  <c:v>0.72363280000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68200000000000005</c:v>
+                  <c:v>0.66816639999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.63800000000000001</c:v>
+                  <c:v>0.61325359999999984</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.59400000000000008</c:v>
+                  <c:v>0.57124719999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.55449999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8494,37 +8501,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.8</c:v>
+                  <c:v>0.76800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.78799999999999992</c:v>
+                  <c:v>0.76170880000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.77600000000000002</c:v>
+                  <c:v>0.75664639999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76400000000000001</c:v>
+                  <c:v>0.75096960000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.752</c:v>
+                  <c:v>0.74283519999999992</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.74</c:v>
+                  <c:v>0.73040000000000016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.71199999999999997</c:v>
+                  <c:v>0.70877440000000014</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68400000000000005</c:v>
+                  <c:v>0.67918719999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.65600000000000003</c:v>
+                  <c:v>0.64897280000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.628</c:v>
+                  <c:v>0.62546559999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.6</c:v>
+                  <c:v>0.6160000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8747,6 +8754,1564 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$L$5:$L$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.504</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15300000000000008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.1999999999999981E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8999999999999989E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$M$5:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.96160000000000012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.86768560000000017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76170880000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64883920000000006</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.53424640000000012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.42310000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32056960000000007</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23182480000000011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16203519999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1163704</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$N$5:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.92479999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.84579680000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75664639999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6616976</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5652992</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4718</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38554879999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.31089440000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25218560000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21377119999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.19999999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$O$5:$O$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.8872000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82319520000000013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75096960000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67404640000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59594880000000017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.52020000000000011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.45032320000000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.38984160000000012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34227840000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.31115680000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$P$5:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.84640000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.79774240000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74283519999999992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6843568000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62498560000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56740000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.51427840000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.46829920000000008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.43214080000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4084816</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$Q$5:$Q$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76730000000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.73040000000000016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69110000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65120000000000011</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61250000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57679999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.54590000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52159999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.50569999999999993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$R$5:$R$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.73680000000000012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.72363280000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70877440000000014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69294960000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67688320000000013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66130000000000011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64692480000000008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.63448240000000011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.62469760000000008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.61829520000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.6160000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$S$5:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.65839999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.66816639999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67918719999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69092480000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70284159999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71440000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7250624</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.73429120000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.74154880000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.74629759999999989</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.748</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$T$5:$T$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.58159999999999989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61325359999999984</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64897280000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68701520000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72563839999999991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7631</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.79765760000000008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8275688000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.85109120000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8664824000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.87200000000000011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$U$5:$U$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5232</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57124719999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.62546559999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6832104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74183679999999985</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.79870000000000008</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8511552</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.89655759999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.93226240000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.95562479999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.96399999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Interpolaton2D!$V$5:$V$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.55449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74799999999999989</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.87200000000000011</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99049999999999994</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-3810-48C7-BCB7-7DCAE5E5403E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1290548111"/>
+        <c:axId val="1290548527"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1290548111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1290548527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1290548527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1290548111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -8787,7 +10352,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9438,16 +11559,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>121104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>616403</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>26535</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9468,15 +11589,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>54768</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>43882</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>179614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>635793</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:colOff>1311728</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -9491,6 +11612,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>106136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>209549</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>73479</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9810,7 +11961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U132"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
@@ -16945,8 +19096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -16964,7 +19115,7 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>30</v>
@@ -16981,7 +19132,7 @@
       </c>
       <c r="I4" s="6" t="str">
         <f>_xll.acq_interpolator2d_create(D5:F5,C6:C7,D6:F7,I3)</f>
-        <v>#acqInterpolator2D:0</v>
+        <v>#acqInterpolator2D:5</v>
       </c>
       <c r="L4" s="15">
         <v>0</v>
@@ -17039,19 +19190,19 @@
       </c>
       <c r="M5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K5)</f>
-        <v>0.96</v>
+        <v>0.96160000000000012</v>
       </c>
       <c r="N5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K5)</f>
-        <v>0.92</v>
+        <v>0.92479999999999996</v>
       </c>
       <c r="O5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K5)</f>
-        <v>0.88</v>
+        <v>0.8872000000000001</v>
       </c>
       <c r="P5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K5)</f>
-        <v>0.84000000000000008</v>
+        <v>0.84640000000000004</v>
       </c>
       <c r="Q5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K5)</f>
@@ -17059,26 +19210,26 @@
       </c>
       <c r="R5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K5)</f>
-        <v>0.74</v>
+        <v>0.73680000000000012</v>
       </c>
       <c r="S5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K5)</f>
-        <v>0.68</v>
+        <v>0.65839999999999999</v>
       </c>
       <c r="T5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K5)</f>
-        <v>0.62</v>
+        <v>0.58159999999999989</v>
       </c>
       <c r="U5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K5)</f>
-        <v>0.56000000000000005</v>
+        <v>0.5232</v>
       </c>
       <c r="V5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K5)</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="51" t="s">
         <v>29</v>
       </c>
@@ -17094,52 +19245,55 @@
       <c r="F6" s="24">
         <v>0.5</v>
       </c>
+      <c r="H6" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="K6" s="31">
         <v>0.1</v>
       </c>
       <c r="L6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K6)</f>
-        <v>0.9</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="M6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K6)</f>
-        <v>0.874</v>
+        <v>0.86768560000000017</v>
       </c>
       <c r="N6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K6)</f>
-        <v>0.84800000000000009</v>
+        <v>0.84579680000000002</v>
       </c>
       <c r="O6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K6)</f>
-        <v>0.82199999999999995</v>
+        <v>0.82319520000000013</v>
       </c>
       <c r="P6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K6)</f>
-        <v>0.79600000000000004</v>
+        <v>0.79774240000000007</v>
       </c>
       <c r="Q6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K6)</f>
-        <v>0.77</v>
+        <v>0.76730000000000009</v>
       </c>
       <c r="R6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K6)</f>
-        <v>0.72599999999999998</v>
+        <v>0.72363280000000008</v>
       </c>
       <c r="S6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K6)</f>
-        <v>0.68200000000000005</v>
+        <v>0.66816639999999994</v>
       </c>
       <c r="T6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K6)</f>
-        <v>0.63800000000000001</v>
+        <v>0.61325359999999984</v>
       </c>
       <c r="U6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K6)</f>
-        <v>0.59400000000000008</v>
+        <v>0.57124719999999996</v>
       </c>
       <c r="V6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K6)</f>
-        <v>0.55000000000000004</v>
+        <v>0.55449999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -17156,200 +19310,212 @@
       <c r="F7" s="20">
         <v>1</v>
       </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
       <c r="K7" s="31">
         <v>0.2</v>
       </c>
       <c r="L7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K7)</f>
-        <v>0.8</v>
+        <v>0.76800000000000002</v>
       </c>
       <c r="M7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K7)</f>
-        <v>0.78799999999999992</v>
+        <v>0.76170880000000007</v>
       </c>
       <c r="N7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K7)</f>
-        <v>0.77600000000000002</v>
+        <v>0.75664639999999994</v>
       </c>
       <c r="O7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K7)</f>
-        <v>0.76400000000000001</v>
+        <v>0.75096960000000001</v>
       </c>
       <c r="P7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K7)</f>
-        <v>0.752</v>
+        <v>0.74283519999999992</v>
       </c>
       <c r="Q7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K7)</f>
-        <v>0.74</v>
+        <v>0.73040000000000016</v>
       </c>
       <c r="R7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K7)</f>
-        <v>0.71199999999999997</v>
+        <v>0.70877440000000014</v>
       </c>
       <c r="S7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K7)</f>
-        <v>0.68400000000000005</v>
+        <v>0.67918719999999999</v>
       </c>
       <c r="T7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K7)</f>
-        <v>0.65600000000000003</v>
+        <v>0.64897280000000002</v>
       </c>
       <c r="U7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K7)</f>
-        <v>0.628</v>
+        <v>0.62546559999999995</v>
       </c>
       <c r="V7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K7)</f>
-        <v>0.6</v>
+        <v>0.6160000000000001</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B8" s="18"/>
+      <c r="H8" t="s">
+        <v>91</v>
+      </c>
       <c r="K8" s="31">
         <v>0.3</v>
       </c>
       <c r="L8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K8)</f>
-        <v>0.7</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="M8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K8)</f>
-        <v>0.70199999999999996</v>
+        <v>0.64883920000000006</v>
       </c>
       <c r="N8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K8)</f>
-        <v>0.70400000000000007</v>
+        <v>0.6616976</v>
       </c>
       <c r="O8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K8)</f>
-        <v>0.70599999999999996</v>
+        <v>0.67404640000000005</v>
       </c>
       <c r="P8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K8)</f>
-        <v>0.70800000000000007</v>
+        <v>0.6843568000000001</v>
       </c>
       <c r="Q8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K8)</f>
-        <v>0.71000000000000008</v>
+        <v>0.69110000000000005</v>
       </c>
       <c r="R8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K8)</f>
-        <v>0.69799999999999995</v>
+        <v>0.69294960000000005</v>
       </c>
       <c r="S8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K8)</f>
-        <v>0.68600000000000005</v>
+        <v>0.69092480000000001</v>
       </c>
       <c r="T8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K8)</f>
-        <v>0.67400000000000004</v>
+        <v>0.68701520000000005</v>
       </c>
       <c r="U8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K8)</f>
-        <v>0.66200000000000003</v>
+        <v>0.6832104</v>
       </c>
       <c r="V8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K8)</f>
-        <v>0.65</v>
+        <v>0.68149999999999999</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="H9" t="s">
+        <v>92</v>
+      </c>
       <c r="K9" s="31">
         <v>0.4</v>
       </c>
       <c r="L9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K9)</f>
-        <v>0.6</v>
+        <v>0.504</v>
       </c>
       <c r="M9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K9)</f>
-        <v>0.61599999999999988</v>
+        <v>0.53424640000000012</v>
       </c>
       <c r="N9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K9)</f>
-        <v>0.63200000000000012</v>
+        <v>0.5652992</v>
       </c>
       <c r="O9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K9)</f>
-        <v>0.64799999999999991</v>
+        <v>0.59594880000000017</v>
       </c>
       <c r="P9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K9)</f>
-        <v>0.66400000000000003</v>
+        <v>0.62498560000000003</v>
       </c>
       <c r="Q9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K9)</f>
-        <v>0.68</v>
+        <v>0.65120000000000011</v>
       </c>
       <c r="R9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K9)</f>
-        <v>0.68399999999999994</v>
+        <v>0.67688320000000013</v>
       </c>
       <c r="S9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K9)</f>
-        <v>0.68800000000000006</v>
+        <v>0.70284159999999996</v>
       </c>
       <c r="T9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K9)</f>
-        <v>0.69200000000000006</v>
+        <v>0.72563839999999991</v>
       </c>
       <c r="U9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K9)</f>
-        <v>0.69600000000000006</v>
+        <v>0.74183679999999985</v>
       </c>
       <c r="V9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K9)</f>
-        <v>0.7</v>
+        <v>0.74799999999999989</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
       <c r="K10" s="31">
         <v>0.5</v>
       </c>
       <c r="L10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K10)</f>
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="M10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K10)</f>
-        <v>0.53</v>
+        <v>0.42310000000000003</v>
       </c>
       <c r="N10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K10)</f>
-        <v>0.56000000000000005</v>
+        <v>0.4718</v>
       </c>
       <c r="O10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K10)</f>
-        <v>0.59</v>
+        <v>0.52020000000000011</v>
       </c>
       <c r="P10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K10)</f>
-        <v>0.62000000000000011</v>
+        <v>0.56740000000000002</v>
       </c>
       <c r="Q10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K10)</f>
-        <v>0.65</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="R10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K10)</f>
-        <v>0.66999999999999993</v>
+        <v>0.66130000000000011</v>
       </c>
       <c r="S10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K10)</f>
-        <v>0.69</v>
+        <v>0.71440000000000003</v>
       </c>
       <c r="T10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K10)</f>
-        <v>0.71</v>
+        <v>0.7631</v>
       </c>
       <c r="U10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K10)</f>
-        <v>0.73</v>
+        <v>0.79870000000000008</v>
       </c>
       <c r="V10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K10)</f>
-        <v>0.75</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.4">
@@ -17358,47 +19524,47 @@
       </c>
       <c r="L11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K11)</f>
-        <v>0.4</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="M11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K11)</f>
-        <v>0.44399999999999995</v>
+        <v>0.32056960000000007</v>
       </c>
       <c r="N11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K11)</f>
-        <v>0.48800000000000004</v>
+        <v>0.38554879999999997</v>
       </c>
       <c r="O11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K11)</f>
-        <v>0.53200000000000003</v>
+        <v>0.45032320000000009</v>
       </c>
       <c r="P11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K11)</f>
-        <v>0.57600000000000007</v>
+        <v>0.51427840000000002</v>
       </c>
       <c r="Q11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K11)</f>
-        <v>0.62</v>
+        <v>0.57679999999999998</v>
       </c>
       <c r="R11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K11)</f>
-        <v>0.65600000000000003</v>
+        <v>0.64692480000000008</v>
       </c>
       <c r="S11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K11)</f>
-        <v>0.69199999999999995</v>
+        <v>0.7250624</v>
       </c>
       <c r="T11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K11)</f>
-        <v>0.72799999999999998</v>
+        <v>0.79765760000000008</v>
       </c>
       <c r="U11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K11)</f>
-        <v>0.76400000000000001</v>
+        <v>0.8511552</v>
       </c>
       <c r="V11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K11)</f>
-        <v>0.8</v>
+        <v>0.87200000000000011</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.4">
@@ -17407,47 +19573,47 @@
       </c>
       <c r="L12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K12)</f>
-        <v>0.30000000000000004</v>
+        <v>0.15300000000000008</v>
       </c>
       <c r="M12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K12)</f>
-        <v>0.35799999999999998</v>
+        <v>0.23182480000000011</v>
       </c>
       <c r="N12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K12)</f>
-        <v>0.41600000000000004</v>
+        <v>0.31089440000000002</v>
       </c>
       <c r="O12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K12)</f>
-        <v>0.47399999999999998</v>
+        <v>0.38984160000000012</v>
       </c>
       <c r="P12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K12)</f>
-        <v>0.53200000000000003</v>
+        <v>0.46829920000000008</v>
       </c>
       <c r="Q12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K12)</f>
-        <v>0.59000000000000008</v>
+        <v>0.54590000000000005</v>
       </c>
       <c r="R12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K12)</f>
-        <v>0.64200000000000002</v>
+        <v>0.63448240000000011</v>
       </c>
       <c r="S12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K12)</f>
-        <v>0.69399999999999995</v>
+        <v>0.73429120000000003</v>
       </c>
       <c r="T12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K12)</f>
-        <v>0.746</v>
+        <v>0.8275688000000001</v>
       </c>
       <c r="U12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K12)</f>
-        <v>0.79800000000000004</v>
+        <v>0.89655759999999995</v>
       </c>
       <c r="V12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K12)</f>
-        <v>0.85</v>
+        <v>0.92349999999999999</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.4">
@@ -17456,47 +19622,47 @@
       </c>
       <c r="L13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K13)</f>
-        <v>0.19999999999999996</v>
+        <v>7.1999999999999981E-2</v>
       </c>
       <c r="M13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K13)</f>
-        <v>0.27199999999999991</v>
+        <v>0.16203519999999999</v>
       </c>
       <c r="N13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K13)</f>
-        <v>0.34400000000000008</v>
+        <v>0.25218560000000001</v>
       </c>
       <c r="O13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K13)</f>
-        <v>0.41599999999999993</v>
+        <v>0.34227840000000004</v>
       </c>
       <c r="P13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K13)</f>
-        <v>0.48799999999999999</v>
+        <v>0.43214080000000005</v>
       </c>
       <c r="Q13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K13)</f>
-        <v>0.56000000000000005</v>
+        <v>0.52159999999999995</v>
       </c>
       <c r="R13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K13)</f>
-        <v>0.628</v>
+        <v>0.62469760000000008</v>
       </c>
       <c r="S13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K13)</f>
-        <v>0.69599999999999995</v>
+        <v>0.74154880000000001</v>
       </c>
       <c r="T13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K13)</f>
-        <v>0.76400000000000001</v>
+        <v>0.85109120000000005</v>
       </c>
       <c r="U13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K13)</f>
-        <v>0.83200000000000007</v>
+        <v>0.93226240000000005</v>
       </c>
       <c r="V13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K13)</f>
-        <v>0.9</v>
+        <v>0.96399999999999997</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.4">
@@ -17505,47 +19671,47 @@
       </c>
       <c r="L14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K14)</f>
-        <v>9.9999999999999978E-2</v>
+        <v>1.8999999999999989E-2</v>
       </c>
       <c r="M14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K14)</f>
-        <v>0.18599999999999994</v>
+        <v>0.1163704</v>
       </c>
       <c r="N14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K14)</f>
-        <v>0.27200000000000002</v>
+        <v>0.21377119999999997</v>
       </c>
       <c r="O14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K14)</f>
-        <v>0.35799999999999987</v>
+        <v>0.31115680000000001</v>
       </c>
       <c r="P14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K14)</f>
-        <v>0.44400000000000001</v>
+        <v>0.4084816</v>
       </c>
       <c r="Q14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K14)</f>
-        <v>0.53</v>
+        <v>0.50569999999999993</v>
       </c>
       <c r="R14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K14)</f>
-        <v>0.61399999999999999</v>
+        <v>0.61829520000000004</v>
       </c>
       <c r="S14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K14)</f>
-        <v>0.69799999999999995</v>
+        <v>0.74629759999999989</v>
       </c>
       <c r="T14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K14)</f>
-        <v>0.78200000000000003</v>
+        <v>0.8664824000000001</v>
       </c>
       <c r="U14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K14)</f>
-        <v>0.8660000000000001</v>
+        <v>0.95562479999999994</v>
       </c>
       <c r="V14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K14)</f>
-        <v>0.95</v>
+        <v>0.99049999999999994</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.4">
@@ -17558,15 +19724,15 @@
       </c>
       <c r="M15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K15)</f>
-        <v>9.9999999999999978E-2</v>
+        <v>0.1</v>
       </c>
       <c r="N15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K15)</f>
-        <v>0.20000000000000007</v>
+        <v>0.19999999999999998</v>
       </c>
       <c r="O15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K15)</f>
-        <v>0.29999999999999993</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="P15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K15)</f>
@@ -17578,19 +19744,19 @@
       </c>
       <c r="R15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K15)</f>
-        <v>0.6</v>
+        <v>0.6160000000000001</v>
       </c>
       <c r="S15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K15)</f>
-        <v>0.7</v>
+        <v>0.748</v>
       </c>
       <c r="T15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K15)</f>
-        <v>0.8</v>
+        <v>0.87200000000000011</v>
       </c>
       <c r="U15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K15)</f>
-        <v>0.9</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="V15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K15)</f>
@@ -17604,507 +19770,507 @@
     </row>
     <row r="18" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L18" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <f>_xll.acq_interpolation2d(L$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
         <v>1</v>
       </c>
       <c r="M18" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.96</v>
+        <f>_xll.acq_interpolation2d(M$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.96160000000000012</v>
       </c>
       <c r="N18" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.92</v>
+        <f>_xll.acq_interpolation2d(N$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.92479999999999996</v>
       </c>
       <c r="O18" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.88</v>
+        <f>_xll.acq_interpolation2d(O$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.8872000000000001</v>
       </c>
       <c r="P18" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.84000000000000008</v>
+        <f>_xll.acq_interpolation2d(P$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.84640000000000004</v>
       </c>
       <c r="Q18" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <f>_xll.acq_interpolation2d(Q$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
         <v>0.8</v>
       </c>
       <c r="R18" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.74</v>
+        <f>_xll.acq_interpolation2d(R$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.73680000000000012</v>
       </c>
       <c r="S18" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.68</v>
+        <f>_xll.acq_interpolation2d(S$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.65839999999999999</v>
       </c>
       <c r="T18" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.62</v>
+        <f>_xll.acq_interpolation2d(T$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.58159999999999989</v>
       </c>
       <c r="U18" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.56000000000000005</v>
+        <f>_xll.acq_interpolation2d(U$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.5232</v>
       </c>
       <c r="V18" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <f>_xll.acq_interpolation2d(V$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L19" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.9</v>
+        <f>_xll.acq_interpolation2d(L$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.89100000000000001</v>
       </c>
       <c r="M19" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.874</v>
+        <f>_xll.acq_interpolation2d(M$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.86768560000000017</v>
       </c>
       <c r="N19" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.84800000000000009</v>
+        <f>_xll.acq_interpolation2d(N$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.84579680000000002</v>
       </c>
       <c r="O19" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.82199999999999995</v>
+        <f>_xll.acq_interpolation2d(O$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.82319520000000013</v>
       </c>
       <c r="P19" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.79600000000000004</v>
+        <f>_xll.acq_interpolation2d(P$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.79774240000000007</v>
       </c>
       <c r="Q19" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.77</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.76730000000000009</v>
       </c>
       <c r="R19" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.72599999999999998</v>
+        <f>_xll.acq_interpolation2d(R$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.72363280000000008</v>
       </c>
       <c r="S19" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.68200000000000005</v>
+        <f>_xll.acq_interpolation2d(S$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.66816639999999994</v>
       </c>
       <c r="T19" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.63800000000000001</v>
+        <f>_xll.acq_interpolation2d(T$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.61325359999999984</v>
       </c>
       <c r="U19" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.59400000000000008</v>
+        <f>_xll.acq_interpolation2d(U$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.57124719999999996</v>
       </c>
       <c r="V19" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.55000000000000004</v>
+        <f>_xll.acq_interpolation2d(V$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.55449999999999999</v>
       </c>
     </row>
     <row r="20" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L20" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.8</v>
+        <f>_xll.acq_interpolation2d(L$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.76800000000000002</v>
       </c>
       <c r="M20" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.78799999999999992</v>
+        <f>_xll.acq_interpolation2d(M$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.76170880000000007</v>
       </c>
       <c r="N20" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.77600000000000002</v>
+        <f>_xll.acq_interpolation2d(N$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.75664639999999994</v>
       </c>
       <c r="O20" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.76400000000000001</v>
+        <f>_xll.acq_interpolation2d(O$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.75096960000000001</v>
       </c>
       <c r="P20" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.752</v>
+        <f>_xll.acq_interpolation2d(P$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.74283519999999992</v>
       </c>
       <c r="Q20" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.74</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.73040000000000016</v>
       </c>
       <c r="R20" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.71199999999999997</v>
+        <f>_xll.acq_interpolation2d(R$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.70877440000000014</v>
       </c>
       <c r="S20" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.68400000000000005</v>
+        <f>_xll.acq_interpolation2d(S$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.67918719999999999</v>
       </c>
       <c r="T20" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.65600000000000003</v>
+        <f>_xll.acq_interpolation2d(T$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.64897280000000002</v>
       </c>
       <c r="U20" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.628</v>
+        <f>_xll.acq_interpolation2d(U$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.62546559999999995</v>
       </c>
       <c r="V20" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.6</v>
+        <f>_xll.acq_interpolation2d(V$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.6160000000000001</v>
       </c>
     </row>
     <row r="21" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L21" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.7</v>
+        <f>_xll.acq_interpolation2d(L$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.63700000000000001</v>
       </c>
       <c r="M21" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.70199999999999996</v>
+        <f>_xll.acq_interpolation2d(M$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.64883920000000006</v>
       </c>
       <c r="N21" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.70400000000000007</v>
+        <f>_xll.acq_interpolation2d(N$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.6616976</v>
       </c>
       <c r="O21" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.70599999999999996</v>
+        <f>_xll.acq_interpolation2d(O$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.67404640000000005</v>
       </c>
       <c r="P21" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.70800000000000007</v>
+        <f>_xll.acq_interpolation2d(P$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.6843568000000001</v>
       </c>
       <c r="Q21" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.71000000000000008</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.69110000000000005</v>
       </c>
       <c r="R21" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.69799999999999995</v>
+        <f>_xll.acq_interpolation2d(R$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.69294960000000005</v>
       </c>
       <c r="S21" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.68600000000000005</v>
+        <f>_xll.acq_interpolation2d(S$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.69092480000000001</v>
       </c>
       <c r="T21" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.67400000000000004</v>
+        <f>_xll.acq_interpolation2d(T$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.68701520000000005</v>
       </c>
       <c r="U21" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.66200000000000003</v>
+        <f>_xll.acq_interpolation2d(U$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.6832104</v>
       </c>
       <c r="V21" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.65</v>
+        <f>_xll.acq_interpolation2d(V$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.68149999999999999</v>
       </c>
     </row>
     <row r="22" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L22" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.6</v>
+        <f>_xll.acq_interpolation2d(L$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.504</v>
       </c>
       <c r="M22" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.61599999999999988</v>
+        <f>_xll.acq_interpolation2d(M$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.53424640000000012</v>
       </c>
       <c r="N22" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.63200000000000012</v>
+        <f>_xll.acq_interpolation2d(N$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.5652992</v>
       </c>
       <c r="O22" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.64799999999999991</v>
+        <f>_xll.acq_interpolation2d(O$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.59594880000000017</v>
       </c>
       <c r="P22" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.66400000000000003</v>
+        <f>_xll.acq_interpolation2d(P$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.62498560000000003</v>
       </c>
       <c r="Q22" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.68</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.65120000000000011</v>
       </c>
       <c r="R22" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.68399999999999994</v>
+        <f>_xll.acq_interpolation2d(R$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.67688320000000013</v>
       </c>
       <c r="S22" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.68800000000000006</v>
+        <f>_xll.acq_interpolation2d(S$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.70284159999999996</v>
       </c>
       <c r="T22" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.69200000000000006</v>
+        <f>_xll.acq_interpolation2d(T$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.72563839999999991</v>
       </c>
       <c r="U22" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.69600000000000006</v>
+        <f>_xll.acq_interpolation2d(U$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.74183679999999985</v>
       </c>
       <c r="V22" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.7</v>
+        <f>_xll.acq_interpolation2d(V$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.74799999999999989</v>
       </c>
     </row>
     <row r="23" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L23" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.5</v>
+        <f>_xll.acq_interpolation2d(L$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.375</v>
       </c>
       <c r="M23" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.53</v>
+        <f>_xll.acq_interpolation2d(M$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.42310000000000003</v>
       </c>
       <c r="N23" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.56000000000000005</v>
+        <f>_xll.acq_interpolation2d(N$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.4718</v>
       </c>
       <c r="O23" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.59</v>
+        <f>_xll.acq_interpolation2d(O$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.52020000000000011</v>
       </c>
       <c r="P23" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.62000000000000011</v>
+        <f>_xll.acq_interpolation2d(P$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.56740000000000002</v>
       </c>
       <c r="Q23" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.65</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.61250000000000004</v>
       </c>
       <c r="R23" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.66999999999999993</v>
+        <f>_xll.acq_interpolation2d(R$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.66130000000000011</v>
       </c>
       <c r="S23" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.69</v>
+        <f>_xll.acq_interpolation2d(S$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.71440000000000003</v>
       </c>
       <c r="T23" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.71</v>
+        <f>_xll.acq_interpolation2d(T$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.7631</v>
       </c>
       <c r="U23" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.73</v>
+        <f>_xll.acq_interpolation2d(U$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.79870000000000008</v>
       </c>
       <c r="V23" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.75</v>
+        <f>_xll.acq_interpolation2d(V$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="24" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L24" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.4</v>
+        <f>_xll.acq_interpolation2d(L$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.25600000000000001</v>
       </c>
       <c r="M24" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.44399999999999995</v>
+        <f>_xll.acq_interpolation2d(M$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.32056960000000007</v>
       </c>
       <c r="N24" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.48800000000000004</v>
+        <f>_xll.acq_interpolation2d(N$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.38554879999999997</v>
       </c>
       <c r="O24" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.53200000000000003</v>
+        <f>_xll.acq_interpolation2d(O$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.45032320000000009</v>
       </c>
       <c r="P24" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.57600000000000007</v>
+        <f>_xll.acq_interpolation2d(P$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.51427840000000002</v>
       </c>
       <c r="Q24" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.62</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.57679999999999998</v>
       </c>
       <c r="R24" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.65600000000000003</v>
+        <f>_xll.acq_interpolation2d(R$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.64692480000000008</v>
       </c>
       <c r="S24" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.69199999999999995</v>
+        <f>_xll.acq_interpolation2d(S$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.7250624</v>
       </c>
       <c r="T24" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.72799999999999998</v>
+        <f>_xll.acq_interpolation2d(T$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.79765760000000008</v>
       </c>
       <c r="U24" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.76400000000000001</v>
+        <f>_xll.acq_interpolation2d(U$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.8511552</v>
       </c>
       <c r="V24" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.8</v>
+        <f>_xll.acq_interpolation2d(V$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.87200000000000011</v>
       </c>
     </row>
     <row r="25" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L25" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.30000000000000004</v>
+        <f>_xll.acq_interpolation2d(L$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.15300000000000008</v>
       </c>
       <c r="M25" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.35799999999999998</v>
+        <f>_xll.acq_interpolation2d(M$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.23182480000000011</v>
       </c>
       <c r="N25" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.41600000000000004</v>
+        <f>_xll.acq_interpolation2d(N$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.31089440000000002</v>
       </c>
       <c r="O25" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.47399999999999998</v>
+        <f>_xll.acq_interpolation2d(O$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.38984160000000012</v>
       </c>
       <c r="P25" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.53200000000000003</v>
+        <f>_xll.acq_interpolation2d(P$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.46829920000000008</v>
       </c>
       <c r="Q25" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.59000000000000008</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.54590000000000005</v>
       </c>
       <c r="R25" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.64200000000000002</v>
+        <f>_xll.acq_interpolation2d(R$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.63448240000000011</v>
       </c>
       <c r="S25" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.69399999999999995</v>
+        <f>_xll.acq_interpolation2d(S$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.73429120000000003</v>
       </c>
       <c r="T25" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.746</v>
+        <f>_xll.acq_interpolation2d(T$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.8275688000000001</v>
       </c>
       <c r="U25" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.79800000000000004</v>
+        <f>_xll.acq_interpolation2d(U$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.89655759999999995</v>
       </c>
       <c r="V25" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.85</v>
+        <f>_xll.acq_interpolation2d(V$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.92349999999999999</v>
       </c>
     </row>
     <row r="26" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L26" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.19999999999999996</v>
+        <f>_xll.acq_interpolation2d(L$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>7.1999999999999981E-2</v>
       </c>
       <c r="M26" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.27199999999999991</v>
+        <f>_xll.acq_interpolation2d(M$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.16203519999999999</v>
       </c>
       <c r="N26" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.34400000000000008</v>
+        <f>_xll.acq_interpolation2d(N$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.25218560000000001</v>
       </c>
       <c r="O26" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.41599999999999993</v>
+        <f>_xll.acq_interpolation2d(O$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.34227840000000004</v>
       </c>
       <c r="P26" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.48799999999999999</v>
+        <f>_xll.acq_interpolation2d(P$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.43214080000000005</v>
       </c>
       <c r="Q26" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.56000000000000005</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.52159999999999995</v>
       </c>
       <c r="R26" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.628</v>
+        <f>_xll.acq_interpolation2d(R$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.62469760000000008</v>
       </c>
       <c r="S26" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.69599999999999995</v>
+        <f>_xll.acq_interpolation2d(S$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.74154880000000001</v>
       </c>
       <c r="T26" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.76400000000000001</v>
+        <f>_xll.acq_interpolation2d(T$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.85109120000000005</v>
       </c>
       <c r="U26" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.83200000000000007</v>
+        <f>_xll.acq_interpolation2d(U$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.93226240000000005</v>
       </c>
       <c r="V26" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.9</v>
+        <f>_xll.acq_interpolation2d(V$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.96399999999999997</v>
       </c>
     </row>
     <row r="27" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L27" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>9.9999999999999978E-2</v>
+        <f>_xll.acq_interpolation2d(L$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>1.8999999999999989E-2</v>
       </c>
       <c r="M27" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.18599999999999994</v>
+        <f>_xll.acq_interpolation2d(M$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.1163704</v>
       </c>
       <c r="N27" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.27200000000000002</v>
+        <f>_xll.acq_interpolation2d(N$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.21377119999999997</v>
       </c>
       <c r="O27" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.35799999999999987</v>
+        <f>_xll.acq_interpolation2d(O$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.31115680000000001</v>
       </c>
       <c r="P27" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.44400000000000001</v>
+        <f>_xll.acq_interpolation2d(P$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.4084816</v>
       </c>
       <c r="Q27" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.53</v>
+        <f>_xll.acq_interpolation2d(Q$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.50569999999999993</v>
       </c>
       <c r="R27" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.61399999999999999</v>
+        <f>_xll.acq_interpolation2d(R$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.61829520000000004</v>
       </c>
       <c r="S27" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.69799999999999995</v>
+        <f>_xll.acq_interpolation2d(S$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.74629759999999989</v>
       </c>
       <c r="T27" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.78200000000000003</v>
+        <f>_xll.acq_interpolation2d(T$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.8664824000000001</v>
       </c>
       <c r="U27" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.8660000000000001</v>
+        <f>_xll.acq_interpolation2d(U$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.95562479999999994</v>
       </c>
       <c r="V27" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.95</v>
+        <f>_xll.acq_interpolation2d(V$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.99049999999999994</v>
       </c>
     </row>
     <row r="28" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L28" s="16">
-        <f>_xll.acq_interpolation2d(L$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <f>_xll.acq_interpolation2d(L$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
         <v>0</v>
       </c>
       <c r="M28" s="16">
-        <f>_xll.acq_interpolation2d(M$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>9.9999999999999978E-2</v>
+        <f>_xll.acq_interpolation2d(M$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.1</v>
       </c>
       <c r="N28" s="16">
-        <f>_xll.acq_interpolation2d(N$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.20000000000000007</v>
+        <f>_xll.acq_interpolation2d(N$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.19999999999999998</v>
       </c>
       <c r="O28" s="16">
-        <f>_xll.acq_interpolation2d(O$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.29999999999999993</v>
+        <f>_xll.acq_interpolation2d(O$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="P28" s="16">
-        <f>_xll.acq_interpolation2d(P$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <f>_xll.acq_interpolation2d(P$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
         <v>0.4</v>
       </c>
       <c r="Q28" s="16">
-        <f>_xll.acq_interpolation2d(Q$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <f>_xll.acq_interpolation2d(Q$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
         <v>0.5</v>
       </c>
       <c r="R28" s="16">
-        <f>_xll.acq_interpolation2d(R$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.6</v>
+        <f>_xll.acq_interpolation2d(R$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.6160000000000001</v>
       </c>
       <c r="S28" s="16">
-        <f>_xll.acq_interpolation2d(S$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.7</v>
+        <f>_xll.acq_interpolation2d(S$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.748</v>
       </c>
       <c r="T28" s="16">
-        <f>_xll.acq_interpolation2d(T$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.8</v>
+        <f>_xll.acq_interpolation2d(T$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.87200000000000011</v>
       </c>
       <c r="U28" s="16">
-        <f>_xll.acq_interpolation2d(U$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
-        <v>0.9</v>
+        <f>_xll.acq_interpolation2d(U$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
+        <v>0.96399999999999997</v>
       </c>
       <c r="V28" s="16">
-        <f>_xll.acq_interpolation2d(V$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7)</f>
+        <f>_xll.acq_interpolation2d(V$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
         <v>1</v>
       </c>
     </row>
@@ -18113,6 +20279,11 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="D4:F4"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3">
+      <formula1>$H$7:$H$10</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -23606,7 +25777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added biAkima and biHermite interpolations
</commit_message>
<xml_diff>
--- a/Distribution/Demo.xlsx
+++ b/Distribution/Demo.xlsx
@@ -855,7 +855,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -910,6 +910,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -943,14 +945,6 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.a7a04b19a31a4c9eb642676ab37cf19a">
-      <tp t="e">
-        <v>#N/A</v>
-        <stp/>
-        <stp>e79a1697-4349-44b8-ac6d-0b0912bcaa2c</stp>
-        <tr r="I4" s="4"/>
-      </tp>
-    </main>
     <main first="rtdsrv.be1f78f34db74ce1ba29d9b8b6185772">
       <tp t="e">
         <v>#N/A</v>
@@ -966,6 +960,8 @@
         <stp>383aa482-d8e1-4289-873d-6d7cfaf34a0d</stp>
         <tr r="F5" s="2"/>
       </tp>
+    </main>
+    <main first="rtdsrv.666c2edb6b434254be57b404ebf65d1e">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
@@ -980,16 +976,12 @@
         <stp>9a7c33f7-3632-4515-9bfc-15c25b54e5f1</stp>
         <tr r="D8" s="6"/>
       </tp>
-    </main>
-    <main first="rtdsrv.017addb0c58e4917a43bf64c27d6deb9">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
         <stp>3b0febc2-ce1f-4e7e-8a14-104ba3fafea8</stp>
         <tr r="C8" s="6"/>
       </tp>
-    </main>
-    <main first="rtdsrv.017addb0c58e4917a43bf64c27d6deb9">
       <tp t="e">
         <v>#N/A</v>
         <stp/>
@@ -1019,6 +1011,14 @@
         <stp/>
         <stp>3f944f10-1bd0-4fa5-b988-03ff530add35</stp>
         <tr r="O8" s="6"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.0f54d89b7d51427e933b120e10fb588c">
+      <tp t="e">
+        <v>#N/A</v>
+        <stp/>
+        <stp>ebaa4ec6-23c2-4402-a502-341103da7716</stp>
+        <tr r="I4" s="4"/>
       </tp>
     </main>
     <main first="rtdsrv.666c2edb6b434254be57b404ebf65d1e">
@@ -6573,34 +6573,34 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96160000000000012</c:v>
+                  <c:v>0.95947520000000008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92479999999999996</c:v>
+                  <c:v>0.91412479999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8872000000000001</c:v>
+                  <c:v>0.87671680000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.84640000000000004</c:v>
+                  <c:v>0.84773120000000013</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73680000000000012</c:v>
+                  <c:v>0.7231936000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.65839999999999999</c:v>
+                  <c:v>0.63680639999999988</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.58159999999999989</c:v>
+                  <c:v>0.53306239999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5232</c:v>
+                  <c:v>0.41340159999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6682,37 +6682,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.89100000000000001</c:v>
+                  <c:v>0.90000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.86768560000000017</c:v>
+                  <c:v>0.87065280000000012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84579680000000002</c:v>
+                  <c:v>0.84732160000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82319520000000013</c:v>
+                  <c:v>0.8355840000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79774240000000007</c:v>
+                  <c:v>0.82872960000000018</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76730000000000009</c:v>
+                  <c:v>0.7924000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.72363280000000008</c:v>
+                  <c:v>0.68964880000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.66816639999999994</c:v>
+                  <c:v>0.61363199999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61325359999999984</c:v>
+                  <c:v>0.52160079999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57124719999999996</c:v>
+                  <c:v>0.41242240000000008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55449999999999999</c:v>
+                  <c:v>0.30569999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6794,37 +6794,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.76800000000000002</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76170880000000007</c:v>
+                  <c:v>0.78310400000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75664639999999994</c:v>
+                  <c:v>0.7768832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75096960000000001</c:v>
+                  <c:v>0.78391040000000012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74283519999999992</c:v>
+                  <c:v>0.79447040000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.73040000000000016</c:v>
+                  <c:v>0.77120000000000011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70877440000000014</c:v>
+                  <c:v>0.66008320000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.67918719999999999</c:v>
+                  <c:v>0.59531519999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.64897280000000002</c:v>
+                  <c:v>0.51490559999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.62546559999999995</c:v>
+                  <c:v>0.41727999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.6160000000000001</c:v>
+                  <c:v>0.32159999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6906,37 +6906,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.63700000000000001</c:v>
+                  <c:v>0.70000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64883920000000006</c:v>
+                  <c:v>0.69640640000000009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6616976</c:v>
+                  <c:v>0.70336640000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67404640000000005</c:v>
+                  <c:v>0.72368320000000008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6843568000000001</c:v>
+                  <c:v>0.74787200000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69110000000000005</c:v>
+                  <c:v>0.73880000000000012</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.69294960000000005</c:v>
+                  <c:v>0.63358000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69092480000000001</c:v>
+                  <c:v>0.58090560000000013</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.68701520000000005</c:v>
+                  <c:v>0.51227120000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.6832104</c:v>
+                  <c:v>0.42718719999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.68149999999999999</c:v>
+                  <c:v>0.34589999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7018,37 +7018,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.504</c:v>
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.53424640000000012</c:v>
+                  <c:v>0.61013759999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5652992</c:v>
+                  <c:v>0.627328</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.59594880000000017</c:v>
+                  <c:v>0.65688960000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.62498560000000003</c:v>
+                  <c:v>0.69185280000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.65120000000000011</c:v>
+                  <c:v>0.69760000000000011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67688320000000013</c:v>
+                  <c:v>0.60922239999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.70284159999999996</c:v>
+                  <c:v>0.56945280000000009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.72563839999999991</c:v>
+                  <c:v>0.51299199999999989</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.74183679999999985</c:v>
+                  <c:v>0.44135679999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74799999999999989</c:v>
+                  <c:v>0.37679999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7130,37 +7130,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.375</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.42310000000000003</c:v>
+                  <c:v>0.5238752000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4718</c:v>
+                  <c:v>0.54932480000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52020000000000011</c:v>
+                  <c:v>0.58551680000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.56740000000000002</c:v>
+                  <c:v>0.62933120000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.61250000000000004</c:v>
+                  <c:v>0.65000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.66130000000000011</c:v>
+                  <c:v>0.58609360000000021</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.71440000000000003</c:v>
+                  <c:v>0.5600063999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.7631</c:v>
+                  <c:v>0.5163624</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79870000000000008</c:v>
+                  <c:v>0.45900159999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.8125</c:v>
+                  <c:v>0.41249999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7244,37 +7244,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.25600000000000001</c:v>
+                  <c:v>0.39999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32056960000000007</c:v>
+                  <c:v>0.4371968</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.38554879999999997</c:v>
+                  <c:v>0.46991359999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45032320000000009</c:v>
+                  <c:v>0.51155200000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51427840000000002</c:v>
+                  <c:v>0.56322559999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57679999999999998</c:v>
+                  <c:v>0.59840000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.64692480000000008</c:v>
+                  <c:v>0.56327680000000013</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7250624</c:v>
+                  <c:v>0.55161600000000011</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79765760000000008</c:v>
+                  <c:v>0.52167679999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8511552</c:v>
+                  <c:v>0.47933439999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.87200000000000011</c:v>
+                  <c:v>0.45119999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7358,37 +7358,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.15300000000000008</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.23182480000000011</c:v>
+                  <c:v>0.3496800000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31089440000000002</c:v>
+                  <c:v>0.38965120000000009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38984160000000012</c:v>
+                  <c:v>0.43698240000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46829920000000008</c:v>
+                  <c:v>0.49645440000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.54590000000000005</c:v>
+                  <c:v>0.54520000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.63448240000000011</c:v>
+                  <c:v>0.53985520000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.73429120000000003</c:v>
+                  <c:v>0.54333120000000013</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8275688000000001</c:v>
+                  <c:v>0.52822959999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.89655759999999995</c:v>
+                  <c:v>0.50156800000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.92349999999999999</c:v>
+                  <c:v>0.49109999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7472,37 +7472,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>7.1999999999999981E-2</c:v>
+                  <c:v>0.19999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16203519999999999</c:v>
+                  <c:v>0.26090239999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25218560000000001</c:v>
+                  <c:v>0.30909439999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.34227840000000004</c:v>
+                  <c:v>0.36379519999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.43214080000000005</c:v>
+                  <c:v>0.43193599999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.52159999999999995</c:v>
+                  <c:v>0.49280000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.62469760000000008</c:v>
+                  <c:v>0.51491199999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.74154880000000001</c:v>
+                  <c:v>0.53420160000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.85109120000000005</c:v>
+                  <c:v>0.5353152000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.93226240000000005</c:v>
+                  <c:v>0.52491520000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.96399999999999997</c:v>
+                  <c:v>0.53039999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7586,37 +7586,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.8999999999999989E-2</c:v>
+                  <c:v>9.9999999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1163704</c:v>
+                  <c:v>0.17044159999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.21377119999999997</c:v>
+                  <c:v>0.22879999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31115680000000001</c:v>
+                  <c:v>0.29397760000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4084816</c:v>
+                  <c:v>0.3725888</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.50569999999999993</c:v>
+                  <c:v>0.44359999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.61829520000000004</c:v>
+                  <c:v>0.48753039999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.74629759999999989</c:v>
+                  <c:v>0.52327679999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8664824000000001</c:v>
+                  <c:v>0.54222799999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95562479999999994</c:v>
+                  <c:v>0.54858879999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99049999999999994</c:v>
+                  <c:v>0.56729999999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7703,34 +7703,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>7.7875200000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19999999999999998</c:v>
+                  <c:v>0.14932480000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.22951680000000008</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.32133120000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.4</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6160000000000001</c:v>
+                  <c:v>0.45679360000000008</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.748</c:v>
+                  <c:v>0.5096063999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.87200000000000011</c:v>
+                  <c:v>0.54826240000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.96399999999999997</c:v>
+                  <c:v>0.57180159999999991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8270,34 +8270,34 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96160000000000012</c:v>
+                  <c:v>0.95947520000000008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92479999999999996</c:v>
+                  <c:v>0.91412479999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.8872000000000001</c:v>
+                  <c:v>0.87671680000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.84640000000000004</c:v>
+                  <c:v>0.84773120000000013</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.73680000000000012</c:v>
+                  <c:v>0.7231936000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.65839999999999999</c:v>
+                  <c:v>0.63680639999999988</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.58159999999999989</c:v>
+                  <c:v>0.53306239999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5232</c:v>
+                  <c:v>0.41340159999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8384,37 +8384,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.89100000000000001</c:v>
+                  <c:v>0.90000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.86768560000000017</c:v>
+                  <c:v>0.87065280000000012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84579680000000002</c:v>
+                  <c:v>0.84732160000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.82319520000000013</c:v>
+                  <c:v>0.8355840000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79774240000000007</c:v>
+                  <c:v>0.82872960000000018</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.76730000000000009</c:v>
+                  <c:v>0.7924000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.72363280000000008</c:v>
+                  <c:v>0.68964880000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.66816639999999994</c:v>
+                  <c:v>0.61363199999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.61325359999999984</c:v>
+                  <c:v>0.52160079999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.57124719999999996</c:v>
+                  <c:v>0.41242240000000008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55449999999999999</c:v>
+                  <c:v>0.30569999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8501,37 +8501,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.76800000000000002</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76170880000000007</c:v>
+                  <c:v>0.78310400000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75664639999999994</c:v>
+                  <c:v>0.7768832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75096960000000001</c:v>
+                  <c:v>0.78391040000000012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74283519999999992</c:v>
+                  <c:v>0.79447040000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.73040000000000016</c:v>
+                  <c:v>0.77120000000000011</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70877440000000014</c:v>
+                  <c:v>0.66008320000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.67918719999999999</c:v>
+                  <c:v>0.59531519999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.64897280000000002</c:v>
+                  <c:v>0.51490559999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.62546559999999995</c:v>
+                  <c:v>0.41727999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.6160000000000001</c:v>
+                  <c:v>0.32159999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8883,31 +8883,31 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89100000000000001</c:v>
+                  <c:v>0.90000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76800000000000002</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63700000000000001</c:v>
+                  <c:v>0.70000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.504</c:v>
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.375</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25600000000000001</c:v>
+                  <c:v>0.39999999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.15300000000000008</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.1999999999999981E-2</c:v>
+                  <c:v>0.19999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8999999999999989E-2</c:v>
+                  <c:v>9.9999999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -8998,37 +8998,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.96160000000000012</c:v>
+                  <c:v>0.95947520000000008</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.86768560000000017</c:v>
+                  <c:v>0.87065280000000012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76170880000000007</c:v>
+                  <c:v>0.78310400000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64883920000000006</c:v>
+                  <c:v>0.69640640000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53424640000000012</c:v>
+                  <c:v>0.61013759999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.42310000000000003</c:v>
+                  <c:v>0.5238752000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.32056960000000007</c:v>
+                  <c:v>0.4371968</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.23182480000000011</c:v>
+                  <c:v>0.3496800000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16203519999999999</c:v>
+                  <c:v>0.26090239999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1163704</c:v>
+                  <c:v>0.17044159999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1</c:v>
+                  <c:v>7.7875200000000006E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9116,37 +9116,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.92479999999999996</c:v>
+                  <c:v>0.91412479999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.84579680000000002</c:v>
+                  <c:v>0.84732160000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75664639999999994</c:v>
+                  <c:v>0.7768832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6616976</c:v>
+                  <c:v>0.70336640000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5652992</c:v>
+                  <c:v>0.627328</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4718</c:v>
+                  <c:v>0.54932480000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.38554879999999997</c:v>
+                  <c:v>0.46991359999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.31089440000000002</c:v>
+                  <c:v>0.38965120000000009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.25218560000000001</c:v>
+                  <c:v>0.30909439999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.21377119999999997</c:v>
+                  <c:v>0.22879999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.19999999999999998</c:v>
+                  <c:v>0.14932480000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9234,37 +9234,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.8872000000000001</c:v>
+                  <c:v>0.87671680000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82319520000000013</c:v>
+                  <c:v>0.8355840000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.75096960000000001</c:v>
+                  <c:v>0.78391040000000012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67404640000000005</c:v>
+                  <c:v>0.72368320000000008</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.59594880000000017</c:v>
+                  <c:v>0.65688960000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.52020000000000011</c:v>
+                  <c:v>0.58551680000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45032320000000009</c:v>
+                  <c:v>0.51155200000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.38984160000000012</c:v>
+                  <c:v>0.43698240000000005</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.34227840000000004</c:v>
+                  <c:v>0.36379519999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.31115680000000001</c:v>
+                  <c:v>0.29397760000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.22951680000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9352,37 +9352,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.84640000000000004</c:v>
+                  <c:v>0.84773120000000013</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.79774240000000007</c:v>
+                  <c:v>0.82872960000000018</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74283519999999992</c:v>
+                  <c:v>0.79447040000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6843568000000001</c:v>
+                  <c:v>0.74787200000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.62498560000000003</c:v>
+                  <c:v>0.69185280000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56740000000000002</c:v>
+                  <c:v>0.62933120000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51427840000000002</c:v>
+                  <c:v>0.56322559999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.46829920000000008</c:v>
+                  <c:v>0.49645440000000007</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.43214080000000005</c:v>
+                  <c:v>0.43193599999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.4084816</c:v>
+                  <c:v>0.3725888</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4</c:v>
+                  <c:v>0.32133120000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9473,34 +9473,34 @@
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76730000000000009</c:v>
+                  <c:v>0.7924000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73040000000000016</c:v>
+                  <c:v>0.77120000000000011</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69110000000000005</c:v>
+                  <c:v>0.73880000000000012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.65120000000000011</c:v>
+                  <c:v>0.69760000000000011</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.61250000000000004</c:v>
+                  <c:v>0.65000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.57679999999999998</c:v>
+                  <c:v>0.59840000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.54590000000000005</c:v>
+                  <c:v>0.54520000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52159999999999995</c:v>
+                  <c:v>0.49280000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.50569999999999993</c:v>
+                  <c:v>0.44359999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9594,37 +9594,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.73680000000000012</c:v>
+                  <c:v>0.7231936000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72363280000000008</c:v>
+                  <c:v>0.68964880000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.70877440000000014</c:v>
+                  <c:v>0.66008320000000009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69294960000000005</c:v>
+                  <c:v>0.63358000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67688320000000013</c:v>
+                  <c:v>0.60922239999999994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66130000000000011</c:v>
+                  <c:v>0.58609360000000021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.64692480000000008</c:v>
+                  <c:v>0.56327680000000013</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63448240000000011</c:v>
+                  <c:v>0.53985520000000009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.62469760000000008</c:v>
+                  <c:v>0.51491199999999993</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.61829520000000004</c:v>
+                  <c:v>0.48753039999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.6160000000000001</c:v>
+                  <c:v>0.45679360000000008</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9718,37 +9718,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.65839999999999999</c:v>
+                  <c:v>0.63680639999999988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.66816639999999994</c:v>
+                  <c:v>0.61363199999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67918719999999999</c:v>
+                  <c:v>0.59531519999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69092480000000001</c:v>
+                  <c:v>0.58090560000000013</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.70284159999999996</c:v>
+                  <c:v>0.56945280000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.71440000000000003</c:v>
+                  <c:v>0.5600063999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7250624</c:v>
+                  <c:v>0.55161600000000011</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.73429120000000003</c:v>
+                  <c:v>0.54333120000000013</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.74154880000000001</c:v>
+                  <c:v>0.53420160000000005</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.74629759999999989</c:v>
+                  <c:v>0.52327679999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.748</c:v>
+                  <c:v>0.5096063999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9842,37 +9842,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.58159999999999989</c:v>
+                  <c:v>0.53306239999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.61325359999999984</c:v>
+                  <c:v>0.52160079999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64897280000000002</c:v>
+                  <c:v>0.51490559999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.68701520000000005</c:v>
+                  <c:v>0.51227120000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.72563839999999991</c:v>
+                  <c:v>0.51299199999999989</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.7631</c:v>
+                  <c:v>0.5163624</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.79765760000000008</c:v>
+                  <c:v>0.52167679999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8275688000000001</c:v>
+                  <c:v>0.52822959999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.85109120000000005</c:v>
+                  <c:v>0.5353152000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8664824000000001</c:v>
+                  <c:v>0.54222799999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.87200000000000011</c:v>
+                  <c:v>0.54826240000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9966,37 +9966,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.5232</c:v>
+                  <c:v>0.41340159999999992</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57124719999999996</c:v>
+                  <c:v>0.41242240000000008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.62546559999999995</c:v>
+                  <c:v>0.41727999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6832104</c:v>
+                  <c:v>0.42718719999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74183679999999985</c:v>
+                  <c:v>0.44135679999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.79870000000000008</c:v>
+                  <c:v>0.45900159999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8511552</c:v>
+                  <c:v>0.47933439999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.89655759999999995</c:v>
+                  <c:v>0.50156800000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.93226240000000005</c:v>
+                  <c:v>0.52491520000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95562479999999994</c:v>
+                  <c:v>0.54858879999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.96399999999999997</c:v>
+                  <c:v>0.57180159999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10090,37 +10090,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.5</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55449999999999999</c:v>
+                  <c:v>0.30569999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6160000000000001</c:v>
+                  <c:v>0.32159999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.68149999999999999</c:v>
+                  <c:v>0.34589999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74799999999999989</c:v>
+                  <c:v>0.37679999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8125</c:v>
+                  <c:v>0.41249999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.87200000000000011</c:v>
+                  <c:v>0.45119999999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.92349999999999999</c:v>
+                  <c:v>0.49109999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.96399999999999997</c:v>
+                  <c:v>0.53039999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99049999999999994</c:v>
+                  <c:v>0.56729999999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11619,16 +11619,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>106136</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>356506</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>117020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>209549</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>73479</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>84362</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12004,10 +12004,10 @@
       </c>
     </row>
     <row r="2" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="50"/>
+      <c r="C2" s="52"/>
       <c r="M2" t="str">
         <f>_xll.acq_interpolator_create($B$4:$B$16,$C$4:$C$16,M$1,$F$4)</f>
         <v>#acqInterpolator:1</v>
@@ -19094,10 +19094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V28"/>
+  <dimension ref="B2:V40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -19115,18 +19115,18 @@
         <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
       <c r="H4" s="17" t="s">
         <v>1</v>
       </c>
@@ -19184,53 +19184,53 @@
       <c r="K5" s="31">
         <v>0</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="50">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K5)</f>
         <v>1</v>
       </c>
       <c r="M5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K5)</f>
-        <v>0.96160000000000012</v>
+        <v>0.95947520000000008</v>
       </c>
       <c r="N5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K5)</f>
-        <v>0.92479999999999996</v>
+        <v>0.91412479999999996</v>
       </c>
       <c r="O5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K5)</f>
-        <v>0.8872000000000001</v>
+        <v>0.87671680000000007</v>
       </c>
       <c r="P5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K5)</f>
-        <v>0.84640000000000004</v>
-      </c>
-      <c r="Q5" s="16">
+        <v>0.84773120000000013</v>
+      </c>
+      <c r="Q5" s="51">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K5)</f>
         <v>0.8</v>
       </c>
       <c r="R5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K5)</f>
-        <v>0.73680000000000012</v>
+        <v>0.7231936000000001</v>
       </c>
       <c r="S5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K5)</f>
-        <v>0.65839999999999999</v>
+        <v>0.63680639999999988</v>
       </c>
       <c r="T5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K5)</f>
-        <v>0.58159999999999989</v>
+        <v>0.53306239999999994</v>
       </c>
       <c r="U5" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K5)</f>
-        <v>0.5232</v>
-      </c>
-      <c r="V5" s="16">
+        <v>0.41340159999999992</v>
+      </c>
+      <c r="V5" s="51">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K5)</f>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="53" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="28">
@@ -19243,7 +19243,7 @@
         <v>0.8</v>
       </c>
       <c r="F6" s="24">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>3</v>
@@ -19253,51 +19253,51 @@
       </c>
       <c r="L6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K6)</f>
-        <v>0.89100000000000001</v>
+        <v>0.90000000000000013</v>
       </c>
       <c r="M6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K6)</f>
-        <v>0.86768560000000017</v>
+        <v>0.87065280000000012</v>
       </c>
       <c r="N6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K6)</f>
-        <v>0.84579680000000002</v>
+        <v>0.84732160000000001</v>
       </c>
       <c r="O6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K6)</f>
-        <v>0.82319520000000013</v>
+        <v>0.8355840000000001</v>
       </c>
       <c r="P6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K6)</f>
-        <v>0.79774240000000007</v>
+        <v>0.82872960000000018</v>
       </c>
       <c r="Q6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K6)</f>
-        <v>0.76730000000000009</v>
+        <v>0.7924000000000001</v>
       </c>
       <c r="R6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K6)</f>
-        <v>0.72363280000000008</v>
+        <v>0.68964880000000006</v>
       </c>
       <c r="S6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K6)</f>
-        <v>0.66816639999999994</v>
+        <v>0.61363199999999996</v>
       </c>
       <c r="T6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K6)</f>
-        <v>0.61325359999999984</v>
+        <v>0.52160079999999998</v>
       </c>
       <c r="U6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K6)</f>
-        <v>0.57124719999999996</v>
+        <v>0.41242240000000008</v>
       </c>
       <c r="V6" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K6)</f>
-        <v>0.55449999999999999</v>
+        <v>0.30569999999999997</v>
       </c>
     </row>
     <row r="7" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="51"/>
+      <c r="B7" s="53"/>
       <c r="C7" s="29">
         <v>1</v>
       </c>
@@ -19305,10 +19305,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F7" s="20">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="H7" t="s">
         <v>27</v>
@@ -19318,47 +19318,47 @@
       </c>
       <c r="L7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K7)</f>
-        <v>0.76800000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="M7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K7)</f>
-        <v>0.76170880000000007</v>
+        <v>0.78310400000000002</v>
       </c>
       <c r="N7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K7)</f>
-        <v>0.75664639999999994</v>
+        <v>0.7768832</v>
       </c>
       <c r="O7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K7)</f>
-        <v>0.75096960000000001</v>
+        <v>0.78391040000000012</v>
       </c>
       <c r="P7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K7)</f>
-        <v>0.74283519999999992</v>
+        <v>0.79447040000000002</v>
       </c>
       <c r="Q7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K7)</f>
-        <v>0.73040000000000016</v>
+        <v>0.77120000000000011</v>
       </c>
       <c r="R7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K7)</f>
-        <v>0.70877440000000014</v>
+        <v>0.66008320000000009</v>
       </c>
       <c r="S7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K7)</f>
-        <v>0.67918719999999999</v>
+        <v>0.59531519999999993</v>
       </c>
       <c r="T7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K7)</f>
-        <v>0.64897280000000002</v>
+        <v>0.51490559999999996</v>
       </c>
       <c r="U7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K7)</f>
-        <v>0.62546559999999995</v>
+        <v>0.41727999999999998</v>
       </c>
       <c r="V7" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K7)</f>
-        <v>0.6160000000000001</v>
+        <v>0.32159999999999994</v>
       </c>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.4">
@@ -19371,47 +19371,47 @@
       </c>
       <c r="L8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K8)</f>
-        <v>0.63700000000000001</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="M8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K8)</f>
-        <v>0.64883920000000006</v>
+        <v>0.69640640000000009</v>
       </c>
       <c r="N8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K8)</f>
-        <v>0.6616976</v>
+        <v>0.70336640000000006</v>
       </c>
       <c r="O8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K8)</f>
-        <v>0.67404640000000005</v>
+        <v>0.72368320000000008</v>
       </c>
       <c r="P8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K8)</f>
-        <v>0.6843568000000001</v>
+        <v>0.74787200000000009</v>
       </c>
       <c r="Q8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K8)</f>
-        <v>0.69110000000000005</v>
+        <v>0.73880000000000012</v>
       </c>
       <c r="R8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K8)</f>
-        <v>0.69294960000000005</v>
+        <v>0.63358000000000003</v>
       </c>
       <c r="S8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K8)</f>
-        <v>0.69092480000000001</v>
+        <v>0.58090560000000013</v>
       </c>
       <c r="T8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K8)</f>
-        <v>0.68701520000000005</v>
+        <v>0.51227120000000004</v>
       </c>
       <c r="U8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K8)</f>
-        <v>0.6832104</v>
+        <v>0.42718719999999999</v>
       </c>
       <c r="V8" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K8)</f>
-        <v>0.68149999999999999</v>
+        <v>0.34589999999999999</v>
       </c>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.4">
@@ -19423,47 +19423,47 @@
       </c>
       <c r="L9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K9)</f>
-        <v>0.504</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="M9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K9)</f>
-        <v>0.53424640000000012</v>
+        <v>0.61013759999999995</v>
       </c>
       <c r="N9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K9)</f>
-        <v>0.5652992</v>
+        <v>0.627328</v>
       </c>
       <c r="O9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K9)</f>
-        <v>0.59594880000000017</v>
+        <v>0.65688960000000007</v>
       </c>
       <c r="P9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K9)</f>
-        <v>0.62498560000000003</v>
+        <v>0.69185280000000005</v>
       </c>
       <c r="Q9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K9)</f>
-        <v>0.65120000000000011</v>
+        <v>0.69760000000000011</v>
       </c>
       <c r="R9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K9)</f>
-        <v>0.67688320000000013</v>
+        <v>0.60922239999999994</v>
       </c>
       <c r="S9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K9)</f>
-        <v>0.70284159999999996</v>
+        <v>0.56945280000000009</v>
       </c>
       <c r="T9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K9)</f>
-        <v>0.72563839999999991</v>
+        <v>0.51299199999999989</v>
       </c>
       <c r="U9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K9)</f>
-        <v>0.74183679999999985</v>
+        <v>0.44135679999999999</v>
       </c>
       <c r="V9" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K9)</f>
-        <v>0.74799999999999989</v>
+        <v>0.37679999999999997</v>
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.4">
@@ -19475,47 +19475,47 @@
       </c>
       <c r="L10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K10)</f>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="M10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K10)</f>
-        <v>0.42310000000000003</v>
+        <v>0.5238752000000001</v>
       </c>
       <c r="N10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K10)</f>
-        <v>0.4718</v>
+        <v>0.54932480000000006</v>
       </c>
       <c r="O10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K10)</f>
-        <v>0.52020000000000011</v>
+        <v>0.58551680000000006</v>
       </c>
       <c r="P10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K10)</f>
-        <v>0.56740000000000002</v>
+        <v>0.62933120000000009</v>
       </c>
       <c r="Q10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K10)</f>
-        <v>0.61250000000000004</v>
+        <v>0.65000000000000013</v>
       </c>
       <c r="R10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K10)</f>
-        <v>0.66130000000000011</v>
+        <v>0.58609360000000021</v>
       </c>
       <c r="S10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K10)</f>
-        <v>0.71440000000000003</v>
+        <v>0.5600063999999999</v>
       </c>
       <c r="T10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K10)</f>
-        <v>0.7631</v>
+        <v>0.5163624</v>
       </c>
       <c r="U10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K10)</f>
-        <v>0.79870000000000008</v>
+        <v>0.45900159999999995</v>
       </c>
       <c r="V10" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K10)</f>
-        <v>0.8125</v>
+        <v>0.41249999999999998</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.4">
@@ -19524,47 +19524,47 @@
       </c>
       <c r="L11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K11)</f>
-        <v>0.25600000000000001</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="M11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K11)</f>
-        <v>0.32056960000000007</v>
+        <v>0.4371968</v>
       </c>
       <c r="N11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K11)</f>
-        <v>0.38554879999999997</v>
+        <v>0.46991359999999993</v>
       </c>
       <c r="O11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K11)</f>
-        <v>0.45032320000000009</v>
+        <v>0.51155200000000001</v>
       </c>
       <c r="P11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K11)</f>
-        <v>0.51427840000000002</v>
+        <v>0.56322559999999999</v>
       </c>
       <c r="Q11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K11)</f>
-        <v>0.57679999999999998</v>
+        <v>0.59840000000000004</v>
       </c>
       <c r="R11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K11)</f>
-        <v>0.64692480000000008</v>
+        <v>0.56327680000000013</v>
       </c>
       <c r="S11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K11)</f>
-        <v>0.7250624</v>
+        <v>0.55161600000000011</v>
       </c>
       <c r="T11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K11)</f>
-        <v>0.79765760000000008</v>
+        <v>0.52167679999999994</v>
       </c>
       <c r="U11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K11)</f>
-        <v>0.8511552</v>
+        <v>0.47933439999999999</v>
       </c>
       <c r="V11" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K11)</f>
-        <v>0.87200000000000011</v>
+        <v>0.45119999999999993</v>
       </c>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.4">
@@ -19573,47 +19573,47 @@
       </c>
       <c r="L12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K12)</f>
-        <v>0.15300000000000008</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="M12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K12)</f>
-        <v>0.23182480000000011</v>
+        <v>0.3496800000000001</v>
       </c>
       <c r="N12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K12)</f>
-        <v>0.31089440000000002</v>
+        <v>0.38965120000000009</v>
       </c>
       <c r="O12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K12)</f>
-        <v>0.38984160000000012</v>
+        <v>0.43698240000000005</v>
       </c>
       <c r="P12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K12)</f>
-        <v>0.46829920000000008</v>
+        <v>0.49645440000000007</v>
       </c>
       <c r="Q12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K12)</f>
-        <v>0.54590000000000005</v>
+        <v>0.54520000000000002</v>
       </c>
       <c r="R12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K12)</f>
-        <v>0.63448240000000011</v>
+        <v>0.53985520000000009</v>
       </c>
       <c r="S12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K12)</f>
-        <v>0.73429120000000003</v>
+        <v>0.54333120000000013</v>
       </c>
       <c r="T12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K12)</f>
-        <v>0.8275688000000001</v>
+        <v>0.52822959999999997</v>
       </c>
       <c r="U12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K12)</f>
-        <v>0.89655759999999995</v>
+        <v>0.50156800000000001</v>
       </c>
       <c r="V12" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K12)</f>
-        <v>0.92349999999999999</v>
+        <v>0.49109999999999993</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.4">
@@ -19622,47 +19622,47 @@
       </c>
       <c r="L13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K13)</f>
-        <v>7.1999999999999981E-2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="M13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K13)</f>
-        <v>0.16203519999999999</v>
+        <v>0.26090239999999998</v>
       </c>
       <c r="N13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K13)</f>
-        <v>0.25218560000000001</v>
+        <v>0.30909439999999999</v>
       </c>
       <c r="O13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K13)</f>
-        <v>0.34227840000000004</v>
+        <v>0.36379519999999999</v>
       </c>
       <c r="P13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K13)</f>
-        <v>0.43214080000000005</v>
+        <v>0.43193599999999999</v>
       </c>
       <c r="Q13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K13)</f>
-        <v>0.52159999999999995</v>
+        <v>0.49280000000000002</v>
       </c>
       <c r="R13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K13)</f>
-        <v>0.62469760000000008</v>
+        <v>0.51491199999999993</v>
       </c>
       <c r="S13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K13)</f>
-        <v>0.74154880000000001</v>
+        <v>0.53420160000000005</v>
       </c>
       <c r="T13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K13)</f>
-        <v>0.85109120000000005</v>
+        <v>0.5353152000000001</v>
       </c>
       <c r="U13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K13)</f>
-        <v>0.93226240000000005</v>
+        <v>0.52491520000000003</v>
       </c>
       <c r="V13" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K13)</f>
-        <v>0.96399999999999997</v>
+        <v>0.53039999999999998</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.4">
@@ -19671,96 +19671,96 @@
       </c>
       <c r="L14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K14)</f>
-        <v>1.8999999999999989E-2</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="M14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K14)</f>
-        <v>0.1163704</v>
+        <v>0.17044159999999997</v>
       </c>
       <c r="N14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K14)</f>
-        <v>0.21377119999999997</v>
+        <v>0.22879999999999998</v>
       </c>
       <c r="O14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K14)</f>
-        <v>0.31115680000000001</v>
+        <v>0.29397760000000001</v>
       </c>
       <c r="P14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K14)</f>
-        <v>0.4084816</v>
+        <v>0.3725888</v>
       </c>
       <c r="Q14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K14)</f>
-        <v>0.50569999999999993</v>
+        <v>0.44359999999999999</v>
       </c>
       <c r="R14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K14)</f>
-        <v>0.61829520000000004</v>
+        <v>0.48753039999999997</v>
       </c>
       <c r="S14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K14)</f>
-        <v>0.74629759999999989</v>
+        <v>0.52327679999999999</v>
       </c>
       <c r="T14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K14)</f>
-        <v>0.8664824000000001</v>
+        <v>0.54222799999999993</v>
       </c>
       <c r="U14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K14)</f>
-        <v>0.95562479999999994</v>
+        <v>0.54858879999999999</v>
       </c>
       <c r="V14" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K14)</f>
-        <v>0.99049999999999994</v>
+        <v>0.56729999999999992</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.4">
       <c r="K15" s="31">
         <v>1</v>
       </c>
-      <c r="L15" s="16">
+      <c r="L15" s="51">
         <f>_xll.acq_interpolator2d_eval($I$4,L$4,$K15)</f>
         <v>0</v>
       </c>
       <c r="M15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,M$4,$K15)</f>
-        <v>0.1</v>
+        <v>7.7875200000000006E-2</v>
       </c>
       <c r="N15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,N$4,$K15)</f>
-        <v>0.19999999999999998</v>
+        <v>0.14932480000000001</v>
       </c>
       <c r="O15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,O$4,$K15)</f>
-        <v>0.30000000000000004</v>
+        <v>0.22951680000000008</v>
       </c>
       <c r="P15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,P$4,$K15)</f>
+        <v>0.32133120000000004</v>
+      </c>
+      <c r="Q15" s="51">
+        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K15)</f>
         <v>0.4</v>
-      </c>
-      <c r="Q15" s="16">
-        <f>_xll.acq_interpolator2d_eval($I$4,Q$4,$K15)</f>
-        <v>0.5</v>
       </c>
       <c r="R15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,R$4,$K15)</f>
-        <v>0.6160000000000001</v>
+        <v>0.45679360000000008</v>
       </c>
       <c r="S15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,S$4,$K15)</f>
-        <v>0.748</v>
+        <v>0.5096063999999999</v>
       </c>
       <c r="T15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,T$4,$K15)</f>
-        <v>0.87200000000000011</v>
+        <v>0.54826240000000004</v>
       </c>
       <c r="U15" s="16">
         <f>_xll.acq_interpolator2d_eval($I$4,U$4,$K15)</f>
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="V15" s="16">
+        <v>0.57180159999999991</v>
+      </c>
+      <c r="V15" s="51">
         <f>_xll.acq_interpolator2d_eval($I$4,V$4,$K15)</f>
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="17" spans="11:22" x14ac:dyDescent="0.4">
@@ -19775,19 +19775,19 @@
       </c>
       <c r="M18" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.96160000000000012</v>
+        <v>0.95947520000000008</v>
       </c>
       <c r="N18" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.92479999999999996</v>
+        <v>0.91412479999999996</v>
       </c>
       <c r="O18" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.8872000000000001</v>
+        <v>0.87671680000000007</v>
       </c>
       <c r="P18" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.84640000000000004</v>
+        <v>0.84773120000000013</v>
       </c>
       <c r="Q18" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
@@ -19795,437 +19795,437 @@
       </c>
       <c r="R18" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.73680000000000012</v>
+        <v>0.7231936000000001</v>
       </c>
       <c r="S18" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.65839999999999999</v>
+        <v>0.63680639999999988</v>
       </c>
       <c r="T18" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.58159999999999989</v>
+        <v>0.53306239999999994</v>
       </c>
       <c r="U18" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.5232</v>
+        <v>0.41340159999999992</v>
       </c>
       <c r="V18" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K5,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="19" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L19" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.89100000000000001</v>
+        <v>0.90000000000000013</v>
       </c>
       <c r="M19" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.86768560000000017</v>
+        <v>0.87065280000000012</v>
       </c>
       <c r="N19" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.84579680000000002</v>
+        <v>0.84732160000000001</v>
       </c>
       <c r="O19" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.82319520000000013</v>
+        <v>0.8355840000000001</v>
       </c>
       <c r="P19" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.79774240000000007</v>
+        <v>0.82872960000000018</v>
       </c>
       <c r="Q19" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.76730000000000009</v>
+        <v>0.7924000000000001</v>
       </c>
       <c r="R19" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.72363280000000008</v>
+        <v>0.68964880000000006</v>
       </c>
       <c r="S19" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.66816639999999994</v>
+        <v>0.61363199999999996</v>
       </c>
       <c r="T19" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.61325359999999984</v>
+        <v>0.52160079999999998</v>
       </c>
       <c r="U19" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.57124719999999996</v>
+        <v>0.41242240000000008</v>
       </c>
       <c r="V19" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K6,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.55449999999999999</v>
+        <v>0.30569999999999997</v>
       </c>
     </row>
     <row r="20" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L20" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.76800000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="M20" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.76170880000000007</v>
+        <v>0.78310400000000002</v>
       </c>
       <c r="N20" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.75664639999999994</v>
+        <v>0.7768832</v>
       </c>
       <c r="O20" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.75096960000000001</v>
+        <v>0.78391040000000012</v>
       </c>
       <c r="P20" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.74283519999999992</v>
+        <v>0.79447040000000002</v>
       </c>
       <c r="Q20" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.73040000000000016</v>
+        <v>0.77120000000000011</v>
       </c>
       <c r="R20" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.70877440000000014</v>
+        <v>0.66008320000000009</v>
       </c>
       <c r="S20" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.67918719999999999</v>
+        <v>0.59531519999999993</v>
       </c>
       <c r="T20" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.64897280000000002</v>
+        <v>0.51490559999999996</v>
       </c>
       <c r="U20" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.62546559999999995</v>
+        <v>0.41727999999999998</v>
       </c>
       <c r="V20" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K7,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.6160000000000001</v>
+        <v>0.32159999999999994</v>
       </c>
     </row>
     <row r="21" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L21" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.63700000000000001</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="M21" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.64883920000000006</v>
+        <v>0.69640640000000009</v>
       </c>
       <c r="N21" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.6616976</v>
+        <v>0.70336640000000006</v>
       </c>
       <c r="O21" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.67404640000000005</v>
+        <v>0.72368320000000008</v>
       </c>
       <c r="P21" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.6843568000000001</v>
+        <v>0.74787200000000009</v>
       </c>
       <c r="Q21" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.69110000000000005</v>
+        <v>0.73880000000000012</v>
       </c>
       <c r="R21" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.69294960000000005</v>
+        <v>0.63358000000000003</v>
       </c>
       <c r="S21" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.69092480000000001</v>
+        <v>0.58090560000000013</v>
       </c>
       <c r="T21" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.68701520000000005</v>
+        <v>0.51227120000000004</v>
       </c>
       <c r="U21" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.6832104</v>
+        <v>0.42718719999999999</v>
       </c>
       <c r="V21" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K8,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.68149999999999999</v>
+        <v>0.34589999999999999</v>
       </c>
     </row>
     <row r="22" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L22" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.504</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="M22" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.53424640000000012</v>
+        <v>0.61013759999999995</v>
       </c>
       <c r="N22" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.5652992</v>
+        <v>0.627328</v>
       </c>
       <c r="O22" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.59594880000000017</v>
+        <v>0.65688960000000007</v>
       </c>
       <c r="P22" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.62498560000000003</v>
+        <v>0.69185280000000005</v>
       </c>
       <c r="Q22" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.65120000000000011</v>
+        <v>0.69760000000000011</v>
       </c>
       <c r="R22" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.67688320000000013</v>
+        <v>0.60922239999999994</v>
       </c>
       <c r="S22" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.70284159999999996</v>
+        <v>0.56945280000000009</v>
       </c>
       <c r="T22" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.72563839999999991</v>
+        <v>0.51299199999999989</v>
       </c>
       <c r="U22" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.74183679999999985</v>
+        <v>0.44135679999999999</v>
       </c>
       <c r="V22" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K9,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.74799999999999989</v>
+        <v>0.37679999999999997</v>
       </c>
     </row>
     <row r="23" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L23" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="M23" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.42310000000000003</v>
+        <v>0.5238752000000001</v>
       </c>
       <c r="N23" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.4718</v>
+        <v>0.54932480000000006</v>
       </c>
       <c r="O23" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.52020000000000011</v>
+        <v>0.58551680000000006</v>
       </c>
       <c r="P23" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.56740000000000002</v>
+        <v>0.62933120000000009</v>
       </c>
       <c r="Q23" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.61250000000000004</v>
+        <v>0.65000000000000013</v>
       </c>
       <c r="R23" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.66130000000000011</v>
+        <v>0.58609360000000021</v>
       </c>
       <c r="S23" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.71440000000000003</v>
+        <v>0.5600063999999999</v>
       </c>
       <c r="T23" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.7631</v>
+        <v>0.5163624</v>
       </c>
       <c r="U23" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.79870000000000008</v>
+        <v>0.45900159999999995</v>
       </c>
       <c r="V23" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K10,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.8125</v>
+        <v>0.41249999999999998</v>
       </c>
     </row>
     <row r="24" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L24" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.25600000000000001</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="M24" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.32056960000000007</v>
+        <v>0.4371968</v>
       </c>
       <c r="N24" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.38554879999999997</v>
+        <v>0.46991359999999993</v>
       </c>
       <c r="O24" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.45032320000000009</v>
+        <v>0.51155200000000001</v>
       </c>
       <c r="P24" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.51427840000000002</v>
+        <v>0.56322559999999999</v>
       </c>
       <c r="Q24" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.57679999999999998</v>
+        <v>0.59840000000000004</v>
       </c>
       <c r="R24" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.64692480000000008</v>
+        <v>0.56327680000000013</v>
       </c>
       <c r="S24" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.7250624</v>
+        <v>0.55161600000000011</v>
       </c>
       <c r="T24" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.79765760000000008</v>
+        <v>0.52167679999999994</v>
       </c>
       <c r="U24" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.8511552</v>
+        <v>0.47933439999999999</v>
       </c>
       <c r="V24" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K11,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.87200000000000011</v>
+        <v>0.45119999999999993</v>
       </c>
     </row>
     <row r="25" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L25" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.15300000000000008</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="M25" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.23182480000000011</v>
+        <v>0.3496800000000001</v>
       </c>
       <c r="N25" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.31089440000000002</v>
+        <v>0.38965120000000009</v>
       </c>
       <c r="O25" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.38984160000000012</v>
+        <v>0.43698240000000005</v>
       </c>
       <c r="P25" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.46829920000000008</v>
+        <v>0.49645440000000007</v>
       </c>
       <c r="Q25" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.54590000000000005</v>
+        <v>0.54520000000000002</v>
       </c>
       <c r="R25" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.63448240000000011</v>
+        <v>0.53985520000000009</v>
       </c>
       <c r="S25" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.73429120000000003</v>
+        <v>0.54333120000000013</v>
       </c>
       <c r="T25" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.8275688000000001</v>
+        <v>0.52822959999999997</v>
       </c>
       <c r="U25" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.89655759999999995</v>
+        <v>0.50156800000000001</v>
       </c>
       <c r="V25" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K12,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.92349999999999999</v>
+        <v>0.49109999999999993</v>
       </c>
     </row>
     <row r="26" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L26" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>7.1999999999999981E-2</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="M26" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.16203519999999999</v>
+        <v>0.26090239999999998</v>
       </c>
       <c r="N26" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.25218560000000001</v>
+        <v>0.30909439999999999</v>
       </c>
       <c r="O26" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.34227840000000004</v>
+        <v>0.36379519999999999</v>
       </c>
       <c r="P26" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.43214080000000005</v>
+        <v>0.43193599999999999</v>
       </c>
       <c r="Q26" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.52159999999999995</v>
+        <v>0.49280000000000002</v>
       </c>
       <c r="R26" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.62469760000000008</v>
+        <v>0.51491199999999993</v>
       </c>
       <c r="S26" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.74154880000000001</v>
+        <v>0.53420160000000005</v>
       </c>
       <c r="T26" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.85109120000000005</v>
+        <v>0.5353152000000001</v>
       </c>
       <c r="U26" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.93226240000000005</v>
+        <v>0.52491520000000003</v>
       </c>
       <c r="V26" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K13,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.96399999999999997</v>
+        <v>0.53039999999999998</v>
       </c>
     </row>
     <row r="27" spans="11:22" x14ac:dyDescent="0.4">
       <c r="L27" s="16">
         <f>_xll.acq_interpolation2d(L$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>1.8999999999999989E-2</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="M27" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.1163704</v>
+        <v>0.17044159999999997</v>
       </c>
       <c r="N27" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.21377119999999997</v>
+        <v>0.22879999999999998</v>
       </c>
       <c r="O27" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.31115680000000001</v>
+        <v>0.29397760000000001</v>
       </c>
       <c r="P27" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.4084816</v>
+        <v>0.3725888</v>
       </c>
       <c r="Q27" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.50569999999999993</v>
+        <v>0.44359999999999999</v>
       </c>
       <c r="R27" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.61829520000000004</v>
+        <v>0.48753039999999997</v>
       </c>
       <c r="S27" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.74629759999999989</v>
+        <v>0.52327679999999999</v>
       </c>
       <c r="T27" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.8664824000000001</v>
+        <v>0.54222799999999993</v>
       </c>
       <c r="U27" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.95562479999999994</v>
+        <v>0.54858879999999999</v>
       </c>
       <c r="V27" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K14,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.99049999999999994</v>
+        <v>0.56729999999999992</v>
       </c>
     </row>
     <row r="28" spans="11:22" x14ac:dyDescent="0.4">
@@ -20235,43 +20235,553 @@
       </c>
       <c r="M28" s="16">
         <f>_xll.acq_interpolation2d(M$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.1</v>
+        <v>7.7875200000000006E-2</v>
       </c>
       <c r="N28" s="16">
         <f>_xll.acq_interpolation2d(N$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.19999999999999998</v>
+        <v>0.14932480000000001</v>
       </c>
       <c r="O28" s="16">
         <f>_xll.acq_interpolation2d(O$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.30000000000000004</v>
+        <v>0.22951680000000008</v>
       </c>
       <c r="P28" s="16">
         <f>_xll.acq_interpolation2d(P$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.4</v>
+        <v>0.32133120000000004</v>
       </c>
       <c r="Q28" s="16">
         <f>_xll.acq_interpolation2d(Q$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R28" s="16">
         <f>_xll.acq_interpolation2d(R$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.6160000000000001</v>
+        <v>0.45679360000000008</v>
       </c>
       <c r="S28" s="16">
         <f>_xll.acq_interpolation2d(S$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.748</v>
+        <v>0.5096063999999999</v>
       </c>
       <c r="T28" s="16">
         <f>_xll.acq_interpolation2d(T$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.87200000000000011</v>
+        <v>0.54826240000000004</v>
       </c>
       <c r="U28" s="16">
         <f>_xll.acq_interpolation2d(U$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>0.96399999999999997</v>
+        <v>0.57180159999999991</v>
       </c>
       <c r="V28" s="16">
         <f>_xll.acq_interpolation2d(V$4,$K15,$D$5:$F$5,$C$6:$C$7,$D$6:$F$7,$I$3)</f>
-        <v>1</v>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="11:22" x14ac:dyDescent="0.4">
+      <c r="K30" s="16">
+        <f>MAX(L30:V40)</f>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f>ABS(L5-L18)</f>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ref="M30:V30" si="0">ABS(M5-M18)</f>
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="11:22" x14ac:dyDescent="0.4">
+      <c r="L31">
+        <f t="shared" ref="L31:V40" si="1">ABS(L6-L19)</f>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="11:22" x14ac:dyDescent="0.4">
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="12:22" x14ac:dyDescent="0.4">
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="12:22" x14ac:dyDescent="0.4">
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="12:22" x14ac:dyDescent="0.4">
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="12:22" x14ac:dyDescent="0.4">
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="12:22" x14ac:dyDescent="0.4">
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="12:22" x14ac:dyDescent="0.4">
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="12:22" x14ac:dyDescent="0.4">
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="12:22" x14ac:dyDescent="0.4">
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>